<commit_message>
lot of new tests images cvs
</commit_message>
<xml_diff>
--- a/csv/results.xlsx
+++ b/csv/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="-15" windowWidth="12030" windowHeight="10275"/>
+    <workbookView xWindow="11985" yWindow="-15" windowWidth="12030" windowHeight="10275" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="89">
   <si>
     <t>case</t>
   </si>
@@ -130,6 +130,159 @@
   </si>
   <si>
     <t>category fps from one text</t>
+  </si>
+  <si>
+    <t>highest similarity</t>
+  </si>
+  <si>
+    <t>worldnews &amp; football</t>
+  </si>
+  <si>
+    <t>fashion &amp; technology</t>
+  </si>
+  <si>
+    <t>film &amp; politics</t>
+  </si>
+  <si>
+    <t>fashion &amp; lifestyle</t>
+  </si>
+  <si>
+    <t>worldnews&amp; football &amp;fashion &amp; lifestyle</t>
+  </si>
+  <si>
+    <t>lifestyle &amp; books &amp;f film &amp; tvandradio</t>
+  </si>
+  <si>
+    <t>worldnews&amp;football&amp;fashion&amp;technology</t>
+  </si>
+  <si>
+    <t>sport &amp; uknews&amp; opinion &amp; society &amp; business</t>
+  </si>
+  <si>
+    <t>politics &amp; worldnews&amp;lifstyle&amp;environment&amp;technology</t>
+  </si>
+  <si>
+    <t>Tv/radio &amp; culture&amp;art/design&amp;film&amp;books</t>
+  </si>
+  <si>
+    <t>UsNews &amp; football&amp; fashion &amp; travel &amp; science</t>
+  </si>
+  <si>
+    <t>Travel&amp;Science</t>
+  </si>
+  <si>
+    <t>Art/design&amp;books&amp;film</t>
+  </si>
+  <si>
+    <t>Business &amp; Politics</t>
+  </si>
+  <si>
+    <t>Politics &amp; Uk News</t>
+  </si>
+  <si>
+    <t>first 10 specific categories</t>
+  </si>
+  <si>
+    <t>second 10 specific categories</t>
+  </si>
+  <si>
+    <t>all categories</t>
+  </si>
+  <si>
+    <t>speed</t>
+  </si>
+  <si>
+    <t>12570 ms</t>
+  </si>
+  <si>
+    <t>11153 ms</t>
+  </si>
+  <si>
+    <t>12060 ms</t>
+  </si>
+  <si>
+    <t>10958 ms</t>
+  </si>
+  <si>
+    <t>13508 ms</t>
+  </si>
+  <si>
+    <t>14467 ms</t>
+  </si>
+  <si>
+    <t>16558 ms</t>
+  </si>
+  <si>
+    <t>14432 ms</t>
+  </si>
+  <si>
+    <t>28699 ms</t>
+  </si>
+  <si>
+    <t>34381 ms</t>
+  </si>
+  <si>
+    <t>16929 ms</t>
+  </si>
+  <si>
+    <t>18137 ms</t>
+  </si>
+  <si>
+    <t>18655 ms</t>
+  </si>
+  <si>
+    <t>19011 ms</t>
+  </si>
+  <si>
+    <t>12554 ms</t>
+  </si>
+  <si>
+    <t>19266 ms</t>
+  </si>
+  <si>
+    <t>12627 ms</t>
+  </si>
+  <si>
+    <t>11274 ms</t>
+  </si>
+  <si>
+    <t>61288 ms</t>
+  </si>
+  <si>
+    <t>427243 ms</t>
+  </si>
+  <si>
+    <t>132605 ms</t>
+  </si>
+  <si>
+    <t>119498 ms</t>
+  </si>
+  <si>
+    <t>42757 ms</t>
+  </si>
+  <si>
+    <t>41373 ms</t>
+  </si>
+  <si>
+    <t>44693 ms</t>
+  </si>
+  <si>
+    <t>50448 ms</t>
+  </si>
+  <si>
+    <t>17256 ms</t>
+  </si>
+  <si>
+    <t>17108 ms</t>
+  </si>
+  <si>
+    <t>32561 ms</t>
+  </si>
+  <si>
+    <t>33050 ms</t>
+  </si>
+  <si>
+    <t>16791 ms</t>
   </si>
 </sst>
 </file>
@@ -153,7 +306,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -213,11 +366,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -239,6 +429,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -544,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C97" workbookViewId="0">
-      <selection activeCell="H114" sqref="H114"/>
+    <sheetView topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:XFD99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3606,13 +3805,1987 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="I56" sqref="I56"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="52.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3">
+        <v>253</v>
+      </c>
+      <c r="D3">
+        <v>50</v>
+      </c>
+      <c r="E3">
+        <v>203</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3">
+        <v>48</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:J20" si="0">I3/D3</f>
+        <v>0.96</v>
+      </c>
+      <c r="K3" t="s">
+        <v>39</v>
+      </c>
+      <c r="L3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>241</v>
+      </c>
+      <c r="D4">
+        <v>48</v>
+      </c>
+      <c r="E4">
+        <f>C4-D4</f>
+        <v>193</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>15</v>
+      </c>
+      <c r="H4" t="s">
+        <v>38</v>
+      </c>
+      <c r="I4">
+        <v>47</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>0.97916666666666663</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>232</v>
+      </c>
+      <c r="D5">
+        <v>46</v>
+      </c>
+      <c r="E5">
+        <f>C5-D5</f>
+        <v>186</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5">
+        <v>15</v>
+      </c>
+      <c r="H5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5">
+        <v>45</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0.97826086956521741</v>
+      </c>
+      <c r="K5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>247</v>
+      </c>
+      <c r="D6">
+        <v>49</v>
+      </c>
+      <c r="E6">
+        <f>C6-D6</f>
+        <v>198</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>38</v>
+      </c>
+      <c r="I6">
+        <v>49</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>42</v>
+      </c>
+      <c r="L6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>500</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>400</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>15</v>
+      </c>
+      <c r="H7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I7">
+        <v>90</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="K7" t="s">
+        <v>43</v>
+      </c>
+      <c r="L7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8">
+        <v>449</v>
+      </c>
+      <c r="D8">
+        <v>89</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:E20" si="1">C8-D8</f>
+        <v>360</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+      <c r="G8">
+        <v>15</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8">
+        <v>75</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>0.84269662921348309</v>
+      </c>
+      <c r="K8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>494</v>
+      </c>
+      <c r="D9">
+        <v>98</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>396</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+      <c r="G9">
+        <v>15</v>
+      </c>
+      <c r="H9" t="s">
+        <v>38</v>
+      </c>
+      <c r="I9">
+        <v>93</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>0.94897959183673475</v>
+      </c>
+      <c r="K9" t="s">
+        <v>45</v>
+      </c>
+      <c r="L9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10">
+        <v>1189</v>
+      </c>
+      <c r="D10">
+        <v>237</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>952</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+      <c r="G10">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>38</v>
+      </c>
+      <c r="I10">
+        <v>165</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>0.69620253164556967</v>
+      </c>
+      <c r="K10" t="s">
+        <v>54</v>
+      </c>
+      <c r="L10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>614</v>
+      </c>
+      <c r="D11">
+        <v>122</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>492</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11">
+        <v>15</v>
+      </c>
+      <c r="H11" t="s">
+        <v>38</v>
+      </c>
+      <c r="I11">
+        <v>106</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>0.86885245901639341</v>
+      </c>
+      <c r="K11" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12">
+        <v>575</v>
+      </c>
+      <c r="D12">
+        <v>115</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>460</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>15</v>
+      </c>
+      <c r="H12" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12">
+        <v>100</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>0.86956521739130432</v>
+      </c>
+      <c r="K12" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
+        <v>517</v>
+      </c>
+      <c r="D13">
+        <v>103</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>414</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13">
+        <v>15</v>
+      </c>
+      <c r="H13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I13">
+        <v>78</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>0.75728155339805825</v>
+      </c>
+      <c r="K13" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>609</v>
+      </c>
+      <c r="D14">
+        <v>121</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>488</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>15</v>
+      </c>
+      <c r="H14" t="s">
+        <v>38</v>
+      </c>
+      <c r="I14">
+        <v>115</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>0.95041322314049592</v>
+      </c>
+      <c r="K14" t="s">
+        <v>49</v>
+      </c>
+      <c r="L14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <v>225</v>
+      </c>
+      <c r="D15">
+        <v>45</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>180</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
+        <v>15</v>
+      </c>
+      <c r="H15" t="s">
+        <v>38</v>
+      </c>
+      <c r="I15">
+        <v>44</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="K15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>301</v>
+      </c>
+      <c r="D16">
+        <v>60</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>241</v>
+      </c>
+      <c r="F16">
+        <v>3</v>
+      </c>
+      <c r="G16">
+        <v>15</v>
+      </c>
+      <c r="H16" t="s">
+        <v>38</v>
+      </c>
+      <c r="I16">
+        <v>57</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>0.95</v>
+      </c>
+      <c r="K16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17">
+        <v>242</v>
+      </c>
+      <c r="D17">
+        <v>48</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>194</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17" t="s">
+        <v>38</v>
+      </c>
+      <c r="I17">
+        <v>43</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>0.89583333333333337</v>
+      </c>
+      <c r="K17" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18">
+        <v>228</v>
+      </c>
+      <c r="D18">
+        <v>45</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>183</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="G18">
+        <v>15</v>
+      </c>
+      <c r="H18" t="s">
+        <v>38</v>
+      </c>
+      <c r="I18">
+        <v>38</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0.84444444444444444</v>
+      </c>
+      <c r="K18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>10</v>
+      </c>
+      <c r="C19">
+        <v>1126</v>
+      </c>
+      <c r="D19">
+        <v>225</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>901</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+      <c r="G19">
+        <v>15</v>
+      </c>
+      <c r="H19" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19">
+        <v>191</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>0.84888888888888892</v>
+      </c>
+      <c r="K19" t="s">
+        <v>55</v>
+      </c>
+      <c r="L19" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20">
+        <v>2315</v>
+      </c>
+      <c r="D20">
+        <v>463</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>1852</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+      <c r="G20">
+        <v>15</v>
+      </c>
+      <c r="H20" t="s">
+        <v>38</v>
+      </c>
+      <c r="I20">
+        <v>318</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>0.68682505399568039</v>
+      </c>
+      <c r="K20" t="s">
+        <v>56</v>
+      </c>
+      <c r="L20" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="24" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="11"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" t="s">
+        <v>4</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" t="s">
+        <v>17</v>
+      </c>
+      <c r="H25" t="s">
+        <v>7</v>
+      </c>
+      <c r="I25" t="s">
+        <v>8</v>
+      </c>
+      <c r="J25" t="s">
+        <v>9</v>
+      </c>
+      <c r="K25" t="s">
+        <v>14</v>
+      </c>
+      <c r="L25" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26">
+        <v>253</v>
+      </c>
+      <c r="D26">
+        <v>50</v>
+      </c>
+      <c r="E26">
+        <f>C26-D26</f>
+        <v>203</v>
+      </c>
+      <c r="F26">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>18</v>
+      </c>
+      <c r="H26" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26">
+        <v>48</v>
+      </c>
+      <c r="J26">
+        <f t="shared" ref="J26:J44" si="2">I26/D26</f>
+        <v>0.96</v>
+      </c>
+      <c r="K26" t="s">
+        <v>39</v>
+      </c>
+      <c r="L26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2</v>
+      </c>
+      <c r="B27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27">
+        <v>241</v>
+      </c>
+      <c r="D27">
+        <v>48</v>
+      </c>
+      <c r="E27">
+        <f>C27-D27</f>
+        <v>193</v>
+      </c>
+      <c r="F27">
+        <v>2</v>
+      </c>
+      <c r="G27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" t="s">
+        <v>19</v>
+      </c>
+      <c r="I27">
+        <v>48</v>
+      </c>
+      <c r="J27">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
+        <v>40</v>
+      </c>
+      <c r="L27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3</v>
+      </c>
+      <c r="B28" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28">
+        <v>232</v>
+      </c>
+      <c r="D28">
+        <v>46</v>
+      </c>
+      <c r="E28">
+        <f>C28-D28</f>
+        <v>186</v>
+      </c>
+      <c r="F28">
+        <v>2</v>
+      </c>
+      <c r="G28" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" t="s">
+        <v>19</v>
+      </c>
+      <c r="I28">
+        <v>44</v>
+      </c>
+      <c r="J28">
+        <f t="shared" si="2"/>
+        <v>0.95652173913043481</v>
+      </c>
+      <c r="K28" t="s">
+        <v>41</v>
+      </c>
+      <c r="L28" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>4</v>
+      </c>
+      <c r="B29" t="s">
+        <v>10</v>
+      </c>
+      <c r="C29">
+        <v>247</v>
+      </c>
+      <c r="D29">
+        <v>49</v>
+      </c>
+      <c r="E29">
+        <f>C29</f>
+        <v>247</v>
+      </c>
+      <c r="F29">
+        <v>2</v>
+      </c>
+      <c r="G29" t="s">
+        <v>18</v>
+      </c>
+      <c r="H29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29">
+        <v>45</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="2"/>
+        <v>0.91836734693877553</v>
+      </c>
+      <c r="K29" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="B30" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30">
+        <v>247</v>
+      </c>
+      <c r="D30">
+        <v>49</v>
+      </c>
+      <c r="E30">
+        <f>C30</f>
+        <v>247</v>
+      </c>
+      <c r="F30">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
+      <c r="I30">
+        <v>45</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="2"/>
+        <v>0.91836734693877553</v>
+      </c>
+      <c r="K30" t="s">
+        <v>42</v>
+      </c>
+      <c r="L30" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>6</v>
+      </c>
+      <c r="B31" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>500</v>
+      </c>
+      <c r="D31">
+        <v>100</v>
+      </c>
+      <c r="E31">
+        <f t="shared" ref="E31:E44" si="3">C31-D31</f>
+        <v>400</v>
+      </c>
+      <c r="F31">
+        <v>4</v>
+      </c>
+      <c r="G31" t="s">
+        <v>18</v>
+      </c>
+      <c r="H31" t="s">
+        <v>19</v>
+      </c>
+      <c r="I31">
+        <v>89</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="2"/>
+        <v>0.89</v>
+      </c>
+      <c r="K31" t="s">
+        <v>43</v>
+      </c>
+      <c r="L31" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>10</v>
+      </c>
+      <c r="C32">
+        <v>449</v>
+      </c>
+      <c r="D32">
+        <v>89</v>
+      </c>
+      <c r="E32">
+        <f t="shared" si="3"/>
+        <v>360</v>
+      </c>
+      <c r="F32">
+        <v>4</v>
+      </c>
+      <c r="G32" t="s">
+        <v>18</v>
+      </c>
+      <c r="H32" t="s">
+        <v>19</v>
+      </c>
+      <c r="I32">
+        <v>70</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="2"/>
+        <v>0.7865168539325843</v>
+      </c>
+      <c r="K32" t="s">
+        <v>44</v>
+      </c>
+      <c r="L32" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>494</v>
+      </c>
+      <c r="D33">
+        <v>98</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="3"/>
+        <v>396</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" t="s">
+        <v>19</v>
+      </c>
+      <c r="I33">
+        <v>92</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="2"/>
+        <v>0.93877551020408168</v>
+      </c>
+      <c r="K33" t="s">
+        <v>45</v>
+      </c>
+      <c r="L33" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>1189</v>
+      </c>
+      <c r="D34">
+        <v>237</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="3"/>
+        <v>952</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="G34" t="s">
+        <v>18</v>
+      </c>
+      <c r="H34" t="s">
+        <v>19</v>
+      </c>
+      <c r="I34">
+        <v>171</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="2"/>
+        <v>0.72151898734177211</v>
+      </c>
+      <c r="K34" t="s">
+        <v>54</v>
+      </c>
+      <c r="L34" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>10</v>
+      </c>
+      <c r="B35" t="s">
+        <v>10</v>
+      </c>
+      <c r="C35">
+        <v>614</v>
+      </c>
+      <c r="D35">
+        <v>122</v>
+      </c>
+      <c r="E35">
+        <f t="shared" si="3"/>
+        <v>492</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+      <c r="G35" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" t="s">
+        <v>19</v>
+      </c>
+      <c r="I35">
+        <v>103</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="2"/>
+        <v>0.84426229508196726</v>
+      </c>
+      <c r="K35" t="s">
+        <v>46</v>
+      </c>
+      <c r="L35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>11</v>
+      </c>
+      <c r="B36" t="s">
+        <v>10</v>
+      </c>
+      <c r="C36">
+        <v>575</v>
+      </c>
+      <c r="D36">
+        <v>115</v>
+      </c>
+      <c r="E36">
+        <f t="shared" si="3"/>
+        <v>460</v>
+      </c>
+      <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="G36" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" t="s">
+        <v>19</v>
+      </c>
+      <c r="I36">
+        <v>101</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="2"/>
+        <v>0.87826086956521743</v>
+      </c>
+      <c r="K36" t="s">
+        <v>47</v>
+      </c>
+      <c r="L36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>517</v>
+      </c>
+      <c r="D37">
+        <v>103</v>
+      </c>
+      <c r="E37">
+        <f t="shared" si="3"/>
+        <v>414</v>
+      </c>
+      <c r="F37">
+        <v>5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" t="s">
+        <v>19</v>
+      </c>
+      <c r="I37">
+        <v>82</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="2"/>
+        <v>0.79611650485436891</v>
+      </c>
+      <c r="K37" t="s">
+        <v>48</v>
+      </c>
+      <c r="L37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>13</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>609</v>
+      </c>
+      <c r="D38">
+        <v>121</v>
+      </c>
+      <c r="E38">
+        <f t="shared" si="3"/>
+        <v>488</v>
+      </c>
+      <c r="F38">
+        <v>5</v>
+      </c>
+      <c r="G38" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" t="s">
+        <v>19</v>
+      </c>
+      <c r="I38">
+        <v>115</v>
+      </c>
+      <c r="J38">
+        <f t="shared" si="2"/>
+        <v>0.95041322314049592</v>
+      </c>
+      <c r="K38" t="s">
+        <v>49</v>
+      </c>
+      <c r="L38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>14</v>
+      </c>
+      <c r="B39" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>225</v>
+      </c>
+      <c r="D39">
+        <v>45</v>
+      </c>
+      <c r="E39">
+        <f t="shared" si="3"/>
+        <v>180</v>
+      </c>
+      <c r="F39">
+        <v>2</v>
+      </c>
+      <c r="G39" t="s">
+        <v>18</v>
+      </c>
+      <c r="H39" t="s">
+        <v>19</v>
+      </c>
+      <c r="I39">
+        <v>44</v>
+      </c>
+      <c r="J39">
+        <f t="shared" si="2"/>
+        <v>0.97777777777777775</v>
+      </c>
+      <c r="K39" t="s">
+        <v>50</v>
+      </c>
+      <c r="L39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>15</v>
+      </c>
+      <c r="B40" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>301</v>
+      </c>
+      <c r="D40">
+        <v>60</v>
+      </c>
+      <c r="E40">
+        <f t="shared" si="3"/>
+        <v>241</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" t="s">
+        <v>19</v>
+      </c>
+      <c r="I40">
+        <v>54</v>
+      </c>
+      <c r="J40">
+        <f t="shared" si="2"/>
+        <v>0.9</v>
+      </c>
+      <c r="K40" t="s">
+        <v>51</v>
+      </c>
+      <c r="L40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>16</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <v>242</v>
+      </c>
+      <c r="D41">
+        <v>48</v>
+      </c>
+      <c r="E41">
+        <f t="shared" si="3"/>
+        <v>194</v>
+      </c>
+      <c r="F41">
+        <v>2</v>
+      </c>
+      <c r="G41" t="s">
+        <v>18</v>
+      </c>
+      <c r="H41" t="s">
+        <v>19</v>
+      </c>
+      <c r="I41">
+        <v>44</v>
+      </c>
+      <c r="J41">
+        <f t="shared" si="2"/>
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="K41" t="s">
+        <v>52</v>
+      </c>
+      <c r="L41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>17</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>228</v>
+      </c>
+      <c r="D42">
+        <v>45</v>
+      </c>
+      <c r="E42">
+        <f t="shared" si="3"/>
+        <v>183</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" t="s">
+        <v>19</v>
+      </c>
+      <c r="I42">
+        <v>39</v>
+      </c>
+      <c r="J42">
+        <f t="shared" si="2"/>
+        <v>0.8666666666666667</v>
+      </c>
+      <c r="K42" t="s">
+        <v>53</v>
+      </c>
+      <c r="L42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>1126</v>
+      </c>
+      <c r="D43">
+        <v>225</v>
+      </c>
+      <c r="E43">
+        <f t="shared" si="3"/>
+        <v>901</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+      <c r="G43" t="s">
+        <v>18</v>
+      </c>
+      <c r="H43" t="s">
+        <v>19</v>
+      </c>
+      <c r="I43">
+        <v>196</v>
+      </c>
+      <c r="J43">
+        <f t="shared" si="2"/>
+        <v>0.87111111111111106</v>
+      </c>
+      <c r="K43" t="s">
+        <v>55</v>
+      </c>
+      <c r="L43" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>19</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>2315</v>
+      </c>
+      <c r="D44">
+        <v>463</v>
+      </c>
+      <c r="E44">
+        <f t="shared" si="3"/>
+        <v>1852</v>
+      </c>
+      <c r="F44">
+        <v>20</v>
+      </c>
+      <c r="G44" t="s">
+        <v>18</v>
+      </c>
+      <c r="H44" t="s">
+        <v>19</v>
+      </c>
+      <c r="I44">
+        <v>349</v>
+      </c>
+      <c r="J44">
+        <f t="shared" si="2"/>
+        <v>0.75377969762419006</v>
+      </c>
+      <c r="K44" t="s">
+        <v>56</v>
+      </c>
+      <c r="L44" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="10"/>
+      <c r="J48" s="10"/>
+      <c r="K48" s="10"/>
+      <c r="L48" s="10"/>
+      <c r="M48" s="11"/>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>0</v>
+      </c>
+      <c r="B49" t="s">
+        <v>1</v>
+      </c>
+      <c r="C49" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" t="s">
+        <v>3</v>
+      </c>
+      <c r="E49" t="s">
+        <v>4</v>
+      </c>
+      <c r="F49" t="s">
+        <v>5</v>
+      </c>
+      <c r="G49" t="s">
+        <v>32</v>
+      </c>
+      <c r="H49" t="s">
+        <v>7</v>
+      </c>
+      <c r="I49" t="s">
+        <v>8</v>
+      </c>
+      <c r="J49" t="s">
+        <v>9</v>
+      </c>
+      <c r="K49" t="s">
+        <v>14</v>
+      </c>
+      <c r="L49" t="s">
+        <v>14</v>
+      </c>
+      <c r="M49" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>253</v>
+      </c>
+      <c r="D50">
+        <v>50</v>
+      </c>
+      <c r="E50">
+        <f>C50-D50</f>
+        <v>203</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="K50" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <v>241</v>
+      </c>
+      <c r="D51">
+        <v>48</v>
+      </c>
+      <c r="E51">
+        <f>C51-D51</f>
+        <v>193</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="K51" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <v>232</v>
+      </c>
+      <c r="D52">
+        <v>46</v>
+      </c>
+      <c r="E52">
+        <f>C52-D52</f>
+        <v>186</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="K52" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <v>247</v>
+      </c>
+      <c r="D53">
+        <v>49</v>
+      </c>
+      <c r="E53">
+        <f>C53-D53</f>
+        <v>198</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="K53" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <v>500</v>
+      </c>
+      <c r="D54">
+        <v>100</v>
+      </c>
+      <c r="E54">
+        <f t="shared" ref="E54:E67" si="4">C54-D54</f>
+        <v>400</v>
+      </c>
+      <c r="F54">
+        <v>4</v>
+      </c>
+      <c r="K54" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <v>449</v>
+      </c>
+      <c r="D55">
+        <v>89</v>
+      </c>
+      <c r="E55">
+        <f t="shared" si="4"/>
+        <v>360</v>
+      </c>
+      <c r="F55">
+        <v>4</v>
+      </c>
+      <c r="K55" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>494</v>
+      </c>
+      <c r="D56">
+        <v>98</v>
+      </c>
+      <c r="E56">
+        <f t="shared" si="4"/>
+        <v>396</v>
+      </c>
+      <c r="F56">
+        <v>4</v>
+      </c>
+      <c r="K56" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>1189</v>
+      </c>
+      <c r="D57">
+        <v>237</v>
+      </c>
+      <c r="E57">
+        <f t="shared" si="4"/>
+        <v>952</v>
+      </c>
+      <c r="F57">
+        <v>10</v>
+      </c>
+      <c r="K57" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <v>614</v>
+      </c>
+      <c r="D58">
+        <v>122</v>
+      </c>
+      <c r="E58">
+        <f t="shared" si="4"/>
+        <v>492</v>
+      </c>
+      <c r="F58">
+        <v>5</v>
+      </c>
+      <c r="K58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>575</v>
+      </c>
+      <c r="D59">
+        <v>115</v>
+      </c>
+      <c r="E59">
+        <f t="shared" si="4"/>
+        <v>460</v>
+      </c>
+      <c r="F59">
+        <v>5</v>
+      </c>
+      <c r="K59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>517</v>
+      </c>
+      <c r="D60">
+        <v>103</v>
+      </c>
+      <c r="E60">
+        <f t="shared" si="4"/>
+        <v>414</v>
+      </c>
+      <c r="F60">
+        <v>5</v>
+      </c>
+      <c r="K60" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>609</v>
+      </c>
+      <c r="D61">
+        <v>121</v>
+      </c>
+      <c r="E61">
+        <f t="shared" si="4"/>
+        <v>488</v>
+      </c>
+      <c r="F61">
+        <v>5</v>
+      </c>
+      <c r="K61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>225</v>
+      </c>
+      <c r="D62">
+        <v>45</v>
+      </c>
+      <c r="E62">
+        <f t="shared" si="4"/>
+        <v>180</v>
+      </c>
+      <c r="F62">
+        <v>2</v>
+      </c>
+      <c r="K62" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>301</v>
+      </c>
+      <c r="D63">
+        <v>60</v>
+      </c>
+      <c r="E63">
+        <f t="shared" si="4"/>
+        <v>241</v>
+      </c>
+      <c r="F63">
+        <v>3</v>
+      </c>
+      <c r="K63" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>242</v>
+      </c>
+      <c r="D64">
+        <v>48</v>
+      </c>
+      <c r="E64">
+        <f t="shared" si="4"/>
+        <v>194</v>
+      </c>
+      <c r="F64">
+        <v>2</v>
+      </c>
+      <c r="K64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>228</v>
+      </c>
+      <c r="D65">
+        <v>45</v>
+      </c>
+      <c r="E65">
+        <f t="shared" si="4"/>
+        <v>183</v>
+      </c>
+      <c r="F65">
+        <v>2</v>
+      </c>
+      <c r="K65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="66" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>1126</v>
+      </c>
+      <c r="D66">
+        <v>225</v>
+      </c>
+      <c r="E66">
+        <f t="shared" si="4"/>
+        <v>901</v>
+      </c>
+      <c r="F66">
+        <v>10</v>
+      </c>
+      <c r="K66" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="67" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>2315</v>
+      </c>
+      <c r="D67">
+        <v>463</v>
+      </c>
+      <c r="E67">
+        <f t="shared" si="4"/>
+        <v>1852</v>
+      </c>
+      <c r="F67">
+        <v>20</v>
+      </c>
+      <c r="K67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="A48:M48"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>